<commit_message>
Changes Website and test sending
Die Zeitanzeige der Website wurde geändert --> Jahresanzeigen oder Monatsanzeigen wurden als unnötig bewertet. Stattdessen wurden 1h, 2Tage und 2Wochen Ansicht eingebaut.

Um diesen Code zu testen, wurde eine Extension in VsCode gefunden, welcher die Codezeilen viel simpler macht, als wenn man es in Arduino schreiben würde. Diese Extension ist wichtig, damit man die Datenübertragung testen kann, ob die gesendeten Werte bei der Website empfangen werden können.
</commit_message>
<xml_diff>
--- a/Sensorbox_HW/Partlist/V2_Partlist_for_7_2_2025.xlsx
+++ b/Sensorbox_HW/Partlist/V2_Partlist_for_7_2_2025.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://htlr-my.sharepoint.com/personal/mert_yilmaz_student_htl-rankweil_at/Documents/Documents/GitHub/DA_Sensorbox/Sensorbox_HW/Partlist/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="840" documentId="11_AD4DB114E441178AC67DF474FE13E1C4693EDF27" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FB6238B7-4B56-4A78-AA3F-C6FF5BF6389C}"/>
+  <xr:revisionPtr revIDLastSave="841" documentId="11_AD4DB114E441178AC67DF474FE13E1C4693EDF27" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{487C8FC9-B0F2-4FCF-915D-DBBAEA74B555}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1052,6 +1052,36 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1061,40 +1091,10 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1384,8 +1384,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D34" zoomScale="93" zoomScaleNormal="53" workbookViewId="0">
-      <selection activeCell="P49" sqref="P49"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="93" zoomScaleNormal="53" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16:W16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1401,56 +1401,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="14.4" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="39"/>
-      <c r="L1" s="39"/>
-      <c r="M1" s="39"/>
-      <c r="N1" s="39"/>
-      <c r="O1" s="39"/>
-      <c r="P1" s="39"/>
-      <c r="Q1" s="39"/>
-      <c r="R1" s="39"/>
-      <c r="S1" s="39"/>
-      <c r="T1" s="39"/>
-      <c r="U1" s="39"/>
-      <c r="V1" s="39"/>
-      <c r="W1" s="39"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="36"/>
+      <c r="P1" s="36"/>
+      <c r="Q1" s="36"/>
+      <c r="R1" s="36"/>
+      <c r="S1" s="36"/>
+      <c r="T1" s="36"/>
+      <c r="U1" s="36"/>
+      <c r="V1" s="36"/>
+      <c r="W1" s="36"/>
     </row>
     <row r="2" spans="1:23" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="40"/>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="40"/>
-      <c r="N2" s="40"/>
-      <c r="O2" s="40"/>
-      <c r="P2" s="40"/>
-      <c r="Q2" s="40"/>
-      <c r="R2" s="40"/>
-      <c r="S2" s="40"/>
-      <c r="T2" s="40"/>
-      <c r="U2" s="40"/>
-      <c r="V2" s="40"/>
-      <c r="W2" s="40"/>
+      <c r="A2" s="37"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="37"/>
+      <c r="O2" s="37"/>
+      <c r="P2" s="37"/>
+      <c r="Q2" s="37"/>
+      <c r="R2" s="37"/>
+      <c r="S2" s="37"/>
+      <c r="T2" s="37"/>
+      <c r="U2" s="37"/>
+      <c r="V2" s="37"/>
+      <c r="W2" s="37"/>
     </row>
     <row r="3" spans="1:23" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
@@ -1477,23 +1477,23 @@
       <c r="H3" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="I3" s="41" t="s">
+      <c r="I3" s="38" t="s">
         <v>114</v>
       </c>
-      <c r="J3" s="41"/>
-      <c r="K3" s="41"/>
-      <c r="L3" s="41"/>
-      <c r="M3" s="41"/>
-      <c r="N3" s="41"/>
-      <c r="O3" s="41"/>
-      <c r="P3" s="41"/>
-      <c r="Q3" s="41"/>
-      <c r="R3" s="41"/>
-      <c r="S3" s="41"/>
-      <c r="T3" s="41"/>
-      <c r="U3" s="41"/>
-      <c r="V3" s="41"/>
-      <c r="W3" s="41"/>
+      <c r="J3" s="38"/>
+      <c r="K3" s="38"/>
+      <c r="L3" s="38"/>
+      <c r="M3" s="38"/>
+      <c r="N3" s="38"/>
+      <c r="O3" s="38"/>
+      <c r="P3" s="38"/>
+      <c r="Q3" s="38"/>
+      <c r="R3" s="38"/>
+      <c r="S3" s="38"/>
+      <c r="T3" s="38"/>
+      <c r="U3" s="38"/>
+      <c r="V3" s="38"/>
+      <c r="W3" s="38"/>
     </row>
     <row r="4" spans="1:23" ht="21" x14ac:dyDescent="0.4">
       <c r="A4" s="17" t="s">
@@ -1520,23 +1520,23 @@
       <c r="H4" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="I4" s="45" t="s">
+      <c r="I4" s="33" t="s">
         <v>170</v>
       </c>
-      <c r="J4" s="45"/>
-      <c r="K4" s="45"/>
-      <c r="L4" s="45"/>
-      <c r="M4" s="45"/>
-      <c r="N4" s="45"/>
-      <c r="O4" s="45"/>
-      <c r="P4" s="45"/>
-      <c r="Q4" s="45"/>
-      <c r="R4" s="45"/>
-      <c r="S4" s="45"/>
-      <c r="T4" s="45"/>
-      <c r="U4" s="45"/>
-      <c r="V4" s="45"/>
-      <c r="W4" s="45"/>
+      <c r="J4" s="33"/>
+      <c r="K4" s="33"/>
+      <c r="L4" s="33"/>
+      <c r="M4" s="33"/>
+      <c r="N4" s="33"/>
+      <c r="O4" s="33"/>
+      <c r="P4" s="33"/>
+      <c r="Q4" s="33"/>
+      <c r="R4" s="33"/>
+      <c r="S4" s="33"/>
+      <c r="T4" s="33"/>
+      <c r="U4" s="33"/>
+      <c r="V4" s="33"/>
+      <c r="W4" s="33"/>
     </row>
     <row r="5" spans="1:23" ht="21" x14ac:dyDescent="0.4">
       <c r="A5" s="19" t="s">
@@ -1562,23 +1562,23 @@
       <c r="H5" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="I5" s="38" t="s">
+      <c r="I5" s="35" t="s">
         <v>122</v>
       </c>
-      <c r="J5" s="38"/>
-      <c r="K5" s="38"/>
-      <c r="L5" s="38"/>
-      <c r="M5" s="38"/>
-      <c r="N5" s="38"/>
-      <c r="O5" s="38"/>
-      <c r="P5" s="38"/>
-      <c r="Q5" s="38"/>
-      <c r="R5" s="38"/>
-      <c r="S5" s="38"/>
-      <c r="T5" s="38"/>
-      <c r="U5" s="38"/>
-      <c r="V5" s="38"/>
-      <c r="W5" s="38"/>
+      <c r="J5" s="35"/>
+      <c r="K5" s="35"/>
+      <c r="L5" s="35"/>
+      <c r="M5" s="35"/>
+      <c r="N5" s="35"/>
+      <c r="O5" s="35"/>
+      <c r="P5" s="35"/>
+      <c r="Q5" s="35"/>
+      <c r="R5" s="35"/>
+      <c r="S5" s="35"/>
+      <c r="T5" s="35"/>
+      <c r="U5" s="35"/>
+      <c r="V5" s="35"/>
+      <c r="W5" s="35"/>
     </row>
     <row r="6" spans="1:23" ht="21" x14ac:dyDescent="0.4">
       <c r="A6" s="19" t="s">
@@ -1606,23 +1606,23 @@
       <c r="H6" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="I6" s="38" t="s">
+      <c r="I6" s="35" t="s">
         <v>116</v>
       </c>
-      <c r="J6" s="38"/>
-      <c r="K6" s="38"/>
-      <c r="L6" s="38"/>
-      <c r="M6" s="38"/>
-      <c r="N6" s="38"/>
-      <c r="O6" s="38"/>
-      <c r="P6" s="38"/>
-      <c r="Q6" s="38"/>
-      <c r="R6" s="38"/>
-      <c r="S6" s="38"/>
-      <c r="T6" s="38"/>
-      <c r="U6" s="38"/>
-      <c r="V6" s="38"/>
-      <c r="W6" s="38"/>
+      <c r="J6" s="35"/>
+      <c r="K6" s="35"/>
+      <c r="L6" s="35"/>
+      <c r="M6" s="35"/>
+      <c r="N6" s="35"/>
+      <c r="O6" s="35"/>
+      <c r="P6" s="35"/>
+      <c r="Q6" s="35"/>
+      <c r="R6" s="35"/>
+      <c r="S6" s="35"/>
+      <c r="T6" s="35"/>
+      <c r="U6" s="35"/>
+      <c r="V6" s="35"/>
+      <c r="W6" s="35"/>
     </row>
     <row r="7" spans="1:23" ht="21" x14ac:dyDescent="0.4">
       <c r="A7" s="19" t="s">
@@ -1650,23 +1650,23 @@
       <c r="H7" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="I7" s="38" t="s">
+      <c r="I7" s="35" t="s">
         <v>121</v>
       </c>
-      <c r="J7" s="38"/>
-      <c r="K7" s="38"/>
-      <c r="L7" s="38"/>
-      <c r="M7" s="38"/>
-      <c r="N7" s="38"/>
-      <c r="O7" s="38"/>
-      <c r="P7" s="38"/>
-      <c r="Q7" s="38"/>
-      <c r="R7" s="38"/>
-      <c r="S7" s="38"/>
-      <c r="T7" s="38"/>
-      <c r="U7" s="38"/>
-      <c r="V7" s="38"/>
-      <c r="W7" s="38"/>
+      <c r="J7" s="35"/>
+      <c r="K7" s="35"/>
+      <c r="L7" s="35"/>
+      <c r="M7" s="35"/>
+      <c r="N7" s="35"/>
+      <c r="O7" s="35"/>
+      <c r="P7" s="35"/>
+      <c r="Q7" s="35"/>
+      <c r="R7" s="35"/>
+      <c r="S7" s="35"/>
+      <c r="T7" s="35"/>
+      <c r="U7" s="35"/>
+      <c r="V7" s="35"/>
+      <c r="W7" s="35"/>
     </row>
     <row r="8" spans="1:23" ht="21" x14ac:dyDescent="0.4">
       <c r="A8" s="19" t="s">
@@ -1694,23 +1694,23 @@
       <c r="H8" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="I8" s="44" t="s">
+      <c r="I8" s="34" t="s">
         <v>172</v>
       </c>
-      <c r="J8" s="44"/>
-      <c r="K8" s="44"/>
-      <c r="L8" s="44"/>
-      <c r="M8" s="44"/>
-      <c r="N8" s="44"/>
-      <c r="O8" s="44"/>
-      <c r="P8" s="44"/>
-      <c r="Q8" s="44"/>
-      <c r="R8" s="44"/>
-      <c r="S8" s="44"/>
-      <c r="T8" s="44"/>
-      <c r="U8" s="44"/>
-      <c r="V8" s="44"/>
-      <c r="W8" s="44"/>
+      <c r="J8" s="34"/>
+      <c r="K8" s="34"/>
+      <c r="L8" s="34"/>
+      <c r="M8" s="34"/>
+      <c r="N8" s="34"/>
+      <c r="O8" s="34"/>
+      <c r="P8" s="34"/>
+      <c r="Q8" s="34"/>
+      <c r="R8" s="34"/>
+      <c r="S8" s="34"/>
+      <c r="T8" s="34"/>
+      <c r="U8" s="34"/>
+      <c r="V8" s="34"/>
+      <c r="W8" s="34"/>
     </row>
     <row r="9" spans="1:23" ht="21" x14ac:dyDescent="0.4">
       <c r="A9" s="19" t="s">
@@ -1738,23 +1738,23 @@
       <c r="H9" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="I9" s="38" t="s">
+      <c r="I9" s="35" t="s">
         <v>124</v>
       </c>
-      <c r="J9" s="38"/>
-      <c r="K9" s="38"/>
-      <c r="L9" s="38"/>
-      <c r="M9" s="38"/>
-      <c r="N9" s="38"/>
-      <c r="O9" s="38"/>
-      <c r="P9" s="38"/>
-      <c r="Q9" s="38"/>
-      <c r="R9" s="38"/>
-      <c r="S9" s="38"/>
-      <c r="T9" s="38"/>
-      <c r="U9" s="38"/>
-      <c r="V9" s="38"/>
-      <c r="W9" s="38"/>
+      <c r="J9" s="35"/>
+      <c r="K9" s="35"/>
+      <c r="L9" s="35"/>
+      <c r="M9" s="35"/>
+      <c r="N9" s="35"/>
+      <c r="O9" s="35"/>
+      <c r="P9" s="35"/>
+      <c r="Q9" s="35"/>
+      <c r="R9" s="35"/>
+      <c r="S9" s="35"/>
+      <c r="T9" s="35"/>
+      <c r="U9" s="35"/>
+      <c r="V9" s="35"/>
+      <c r="W9" s="35"/>
     </row>
     <row r="10" spans="1:23" ht="21" x14ac:dyDescent="0.4">
       <c r="A10" s="19" t="s">
@@ -1782,23 +1782,23 @@
       <c r="H10" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="I10" s="38" t="s">
+      <c r="I10" s="35" t="s">
         <v>127</v>
       </c>
-      <c r="J10" s="38"/>
-      <c r="K10" s="38"/>
-      <c r="L10" s="38"/>
-      <c r="M10" s="38"/>
-      <c r="N10" s="38"/>
-      <c r="O10" s="38"/>
-      <c r="P10" s="38"/>
-      <c r="Q10" s="38"/>
-      <c r="R10" s="38"/>
-      <c r="S10" s="38"/>
-      <c r="T10" s="38"/>
-      <c r="U10" s="38"/>
-      <c r="V10" s="38"/>
-      <c r="W10" s="38"/>
+      <c r="J10" s="35"/>
+      <c r="K10" s="35"/>
+      <c r="L10" s="35"/>
+      <c r="M10" s="35"/>
+      <c r="N10" s="35"/>
+      <c r="O10" s="35"/>
+      <c r="P10" s="35"/>
+      <c r="Q10" s="35"/>
+      <c r="R10" s="35"/>
+      <c r="S10" s="35"/>
+      <c r="T10" s="35"/>
+      <c r="U10" s="35"/>
+      <c r="V10" s="35"/>
+      <c r="W10" s="35"/>
     </row>
     <row r="11" spans="1:23" ht="21" x14ac:dyDescent="0.4">
       <c r="A11" s="19" t="s">
@@ -1826,23 +1826,23 @@
       <c r="H11" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="I11" s="38" t="s">
+      <c r="I11" s="35" t="s">
         <v>129</v>
       </c>
-      <c r="J11" s="38"/>
-      <c r="K11" s="38"/>
-      <c r="L11" s="38"/>
-      <c r="M11" s="38"/>
-      <c r="N11" s="38"/>
-      <c r="O11" s="38"/>
-      <c r="P11" s="38"/>
-      <c r="Q11" s="38"/>
-      <c r="R11" s="38"/>
-      <c r="S11" s="38"/>
-      <c r="T11" s="38"/>
-      <c r="U11" s="38"/>
-      <c r="V11" s="38"/>
-      <c r="W11" s="38"/>
+      <c r="J11" s="35"/>
+      <c r="K11" s="35"/>
+      <c r="L11" s="35"/>
+      <c r="M11" s="35"/>
+      <c r="N11" s="35"/>
+      <c r="O11" s="35"/>
+      <c r="P11" s="35"/>
+      <c r="Q11" s="35"/>
+      <c r="R11" s="35"/>
+      <c r="S11" s="35"/>
+      <c r="T11" s="35"/>
+      <c r="U11" s="35"/>
+      <c r="V11" s="35"/>
+      <c r="W11" s="35"/>
     </row>
     <row r="12" spans="1:23" ht="21" x14ac:dyDescent="0.4">
       <c r="A12" s="19" t="s">
@@ -1870,23 +1870,23 @@
       <c r="H12" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="I12" s="38" t="s">
+      <c r="I12" s="35" t="s">
         <v>131</v>
       </c>
-      <c r="J12" s="38"/>
-      <c r="K12" s="38"/>
-      <c r="L12" s="38"/>
-      <c r="M12" s="38"/>
-      <c r="N12" s="38"/>
-      <c r="O12" s="38"/>
-      <c r="P12" s="38"/>
-      <c r="Q12" s="38"/>
-      <c r="R12" s="38"/>
-      <c r="S12" s="38"/>
-      <c r="T12" s="38"/>
-      <c r="U12" s="38"/>
-      <c r="V12" s="38"/>
-      <c r="W12" s="38"/>
+      <c r="J12" s="35"/>
+      <c r="K12" s="35"/>
+      <c r="L12" s="35"/>
+      <c r="M12" s="35"/>
+      <c r="N12" s="35"/>
+      <c r="O12" s="35"/>
+      <c r="P12" s="35"/>
+      <c r="Q12" s="35"/>
+      <c r="R12" s="35"/>
+      <c r="S12" s="35"/>
+      <c r="T12" s="35"/>
+      <c r="U12" s="35"/>
+      <c r="V12" s="35"/>
+      <c r="W12" s="35"/>
     </row>
     <row r="13" spans="1:23" ht="21" x14ac:dyDescent="0.4">
       <c r="A13" s="19" t="s">
@@ -1914,23 +1914,23 @@
       <c r="H13" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="I13" s="38" t="s">
+      <c r="I13" s="35" t="s">
         <v>133</v>
       </c>
-      <c r="J13" s="38"/>
-      <c r="K13" s="38"/>
-      <c r="L13" s="38"/>
-      <c r="M13" s="38"/>
-      <c r="N13" s="38"/>
-      <c r="O13" s="38"/>
-      <c r="P13" s="38"/>
-      <c r="Q13" s="38"/>
-      <c r="R13" s="38"/>
-      <c r="S13" s="38"/>
-      <c r="T13" s="38"/>
-      <c r="U13" s="38"/>
-      <c r="V13" s="38"/>
-      <c r="W13" s="38"/>
+      <c r="J13" s="35"/>
+      <c r="K13" s="35"/>
+      <c r="L13" s="35"/>
+      <c r="M13" s="35"/>
+      <c r="N13" s="35"/>
+      <c r="O13" s="35"/>
+      <c r="P13" s="35"/>
+      <c r="Q13" s="35"/>
+      <c r="R13" s="35"/>
+      <c r="S13" s="35"/>
+      <c r="T13" s="35"/>
+      <c r="U13" s="35"/>
+      <c r="V13" s="35"/>
+      <c r="W13" s="35"/>
     </row>
     <row r="14" spans="1:23" ht="21" x14ac:dyDescent="0.4">
       <c r="A14" s="19" t="s">
@@ -1958,23 +1958,23 @@
       <c r="H14" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="I14" s="38" t="s">
+      <c r="I14" s="35" t="s">
         <v>135</v>
       </c>
-      <c r="J14" s="38"/>
-      <c r="K14" s="38"/>
-      <c r="L14" s="38"/>
-      <c r="M14" s="38"/>
-      <c r="N14" s="38"/>
-      <c r="O14" s="38"/>
-      <c r="P14" s="38"/>
-      <c r="Q14" s="38"/>
-      <c r="R14" s="38"/>
-      <c r="S14" s="38"/>
-      <c r="T14" s="38"/>
-      <c r="U14" s="38"/>
-      <c r="V14" s="38"/>
-      <c r="W14" s="38"/>
+      <c r="J14" s="35"/>
+      <c r="K14" s="35"/>
+      <c r="L14" s="35"/>
+      <c r="M14" s="35"/>
+      <c r="N14" s="35"/>
+      <c r="O14" s="35"/>
+      <c r="P14" s="35"/>
+      <c r="Q14" s="35"/>
+      <c r="R14" s="35"/>
+      <c r="S14" s="35"/>
+      <c r="T14" s="35"/>
+      <c r="U14" s="35"/>
+      <c r="V14" s="35"/>
+      <c r="W14" s="35"/>
     </row>
     <row r="15" spans="1:23" ht="21" x14ac:dyDescent="0.4">
       <c r="A15" s="19" t="s">
@@ -2002,23 +2002,23 @@
       <c r="H15" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="I15" s="44" t="s">
+      <c r="I15" s="34" t="s">
         <v>174</v>
       </c>
-      <c r="J15" s="44"/>
-      <c r="K15" s="44"/>
-      <c r="L15" s="44"/>
-      <c r="M15" s="44"/>
-      <c r="N15" s="44"/>
-      <c r="O15" s="44"/>
-      <c r="P15" s="44"/>
-      <c r="Q15" s="44"/>
-      <c r="R15" s="44"/>
-      <c r="S15" s="44"/>
-      <c r="T15" s="44"/>
-      <c r="U15" s="44"/>
-      <c r="V15" s="44"/>
-      <c r="W15" s="44"/>
+      <c r="J15" s="34"/>
+      <c r="K15" s="34"/>
+      <c r="L15" s="34"/>
+      <c r="M15" s="34"/>
+      <c r="N15" s="34"/>
+      <c r="O15" s="34"/>
+      <c r="P15" s="34"/>
+      <c r="Q15" s="34"/>
+      <c r="R15" s="34"/>
+      <c r="S15" s="34"/>
+      <c r="T15" s="34"/>
+      <c r="U15" s="34"/>
+      <c r="V15" s="34"/>
+      <c r="W15" s="34"/>
     </row>
     <row r="16" spans="1:23" ht="21" x14ac:dyDescent="0.4">
       <c r="A16" s="19" t="s">
@@ -2046,23 +2046,23 @@
       <c r="H16" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="I16" s="44" t="s">
+      <c r="I16" s="34" t="s">
         <v>175</v>
       </c>
-      <c r="J16" s="44"/>
-      <c r="K16" s="44"/>
-      <c r="L16" s="44"/>
-      <c r="M16" s="44"/>
-      <c r="N16" s="44"/>
-      <c r="O16" s="44"/>
-      <c r="P16" s="44"/>
-      <c r="Q16" s="44"/>
-      <c r="R16" s="44"/>
-      <c r="S16" s="44"/>
-      <c r="T16" s="44"/>
-      <c r="U16" s="44"/>
-      <c r="V16" s="44"/>
-      <c r="W16" s="44"/>
+      <c r="J16" s="34"/>
+      <c r="K16" s="34"/>
+      <c r="L16" s="34"/>
+      <c r="M16" s="34"/>
+      <c r="N16" s="34"/>
+      <c r="O16" s="34"/>
+      <c r="P16" s="34"/>
+      <c r="Q16" s="34"/>
+      <c r="R16" s="34"/>
+      <c r="S16" s="34"/>
+      <c r="T16" s="34"/>
+      <c r="U16" s="34"/>
+      <c r="V16" s="34"/>
+      <c r="W16" s="34"/>
     </row>
     <row r="17" spans="1:23" ht="21" x14ac:dyDescent="0.4">
       <c r="A17" s="19" t="s">
@@ -2087,23 +2087,23 @@
       <c r="H17" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="I17" s="38" t="s">
+      <c r="I17" s="35" t="s">
         <v>137</v>
       </c>
-      <c r="J17" s="38"/>
-      <c r="K17" s="38"/>
-      <c r="L17" s="38"/>
-      <c r="M17" s="38"/>
-      <c r="N17" s="38"/>
-      <c r="O17" s="38"/>
-      <c r="P17" s="38"/>
-      <c r="Q17" s="38"/>
-      <c r="R17" s="38"/>
-      <c r="S17" s="38"/>
-      <c r="T17" s="38"/>
-      <c r="U17" s="38"/>
-      <c r="V17" s="38"/>
-      <c r="W17" s="38"/>
+      <c r="J17" s="35"/>
+      <c r="K17" s="35"/>
+      <c r="L17" s="35"/>
+      <c r="M17" s="35"/>
+      <c r="N17" s="35"/>
+      <c r="O17" s="35"/>
+      <c r="P17" s="35"/>
+      <c r="Q17" s="35"/>
+      <c r="R17" s="35"/>
+      <c r="S17" s="35"/>
+      <c r="T17" s="35"/>
+      <c r="U17" s="35"/>
+      <c r="V17" s="35"/>
+      <c r="W17" s="35"/>
     </row>
     <row r="18" spans="1:23" ht="21" x14ac:dyDescent="0.4">
       <c r="A18" s="19" t="s">
@@ -2131,23 +2131,23 @@
       <c r="H18" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="I18" s="38" t="s">
+      <c r="I18" s="35" t="s">
         <v>141</v>
       </c>
-      <c r="J18" s="38"/>
-      <c r="K18" s="38"/>
-      <c r="L18" s="38"/>
-      <c r="M18" s="38"/>
-      <c r="N18" s="38"/>
-      <c r="O18" s="38"/>
-      <c r="P18" s="38"/>
-      <c r="Q18" s="38"/>
-      <c r="R18" s="38"/>
-      <c r="S18" s="38"/>
-      <c r="T18" s="38"/>
-      <c r="U18" s="38"/>
-      <c r="V18" s="38"/>
-      <c r="W18" s="38"/>
+      <c r="J18" s="35"/>
+      <c r="K18" s="35"/>
+      <c r="L18" s="35"/>
+      <c r="M18" s="35"/>
+      <c r="N18" s="35"/>
+      <c r="O18" s="35"/>
+      <c r="P18" s="35"/>
+      <c r="Q18" s="35"/>
+      <c r="R18" s="35"/>
+      <c r="S18" s="35"/>
+      <c r="T18" s="35"/>
+      <c r="U18" s="35"/>
+      <c r="V18" s="35"/>
+      <c r="W18" s="35"/>
     </row>
     <row r="19" spans="1:23" ht="21" x14ac:dyDescent="0.4">
       <c r="A19" s="19" t="s">
@@ -2175,23 +2175,23 @@
       <c r="H19" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="I19" s="44" t="s">
+      <c r="I19" s="34" t="s">
         <v>177</v>
       </c>
-      <c r="J19" s="44"/>
-      <c r="K19" s="44"/>
-      <c r="L19" s="44"/>
-      <c r="M19" s="44"/>
-      <c r="N19" s="44"/>
-      <c r="O19" s="44"/>
-      <c r="P19" s="44"/>
-      <c r="Q19" s="44"/>
-      <c r="R19" s="44"/>
-      <c r="S19" s="44"/>
-      <c r="T19" s="44"/>
-      <c r="U19" s="44"/>
-      <c r="V19" s="44"/>
-      <c r="W19" s="44"/>
+      <c r="J19" s="34"/>
+      <c r="K19" s="34"/>
+      <c r="L19" s="34"/>
+      <c r="M19" s="34"/>
+      <c r="N19" s="34"/>
+      <c r="O19" s="34"/>
+      <c r="P19" s="34"/>
+      <c r="Q19" s="34"/>
+      <c r="R19" s="34"/>
+      <c r="S19" s="34"/>
+      <c r="T19" s="34"/>
+      <c r="U19" s="34"/>
+      <c r="V19" s="34"/>
+      <c r="W19" s="34"/>
     </row>
     <row r="20" spans="1:23" ht="21" x14ac:dyDescent="0.4">
       <c r="A20" s="19" t="s">
@@ -2219,23 +2219,23 @@
       <c r="H20" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="I20" s="38" t="s">
+      <c r="I20" s="35" t="s">
         <v>143</v>
       </c>
-      <c r="J20" s="38"/>
-      <c r="K20" s="38"/>
-      <c r="L20" s="38"/>
-      <c r="M20" s="38"/>
-      <c r="N20" s="38"/>
-      <c r="O20" s="38"/>
-      <c r="P20" s="38"/>
-      <c r="Q20" s="38"/>
-      <c r="R20" s="38"/>
-      <c r="S20" s="38"/>
-      <c r="T20" s="38"/>
-      <c r="U20" s="38"/>
-      <c r="V20" s="38"/>
-      <c r="W20" s="38"/>
+      <c r="J20" s="35"/>
+      <c r="K20" s="35"/>
+      <c r="L20" s="35"/>
+      <c r="M20" s="35"/>
+      <c r="N20" s="35"/>
+      <c r="O20" s="35"/>
+      <c r="P20" s="35"/>
+      <c r="Q20" s="35"/>
+      <c r="R20" s="35"/>
+      <c r="S20" s="35"/>
+      <c r="T20" s="35"/>
+      <c r="U20" s="35"/>
+      <c r="V20" s="35"/>
+      <c r="W20" s="35"/>
     </row>
     <row r="21" spans="1:23" ht="21" x14ac:dyDescent="0.4">
       <c r="A21" s="19" t="s">
@@ -2263,23 +2263,23 @@
       <c r="H21" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="I21" s="38" t="s">
+      <c r="I21" s="35" t="s">
         <v>145</v>
       </c>
-      <c r="J21" s="38"/>
-      <c r="K21" s="38"/>
-      <c r="L21" s="38"/>
-      <c r="M21" s="38"/>
-      <c r="N21" s="38"/>
-      <c r="O21" s="38"/>
-      <c r="P21" s="38"/>
-      <c r="Q21" s="38"/>
-      <c r="R21" s="38"/>
-      <c r="S21" s="38"/>
-      <c r="T21" s="38"/>
-      <c r="U21" s="38"/>
-      <c r="V21" s="38"/>
-      <c r="W21" s="38"/>
+      <c r="J21" s="35"/>
+      <c r="K21" s="35"/>
+      <c r="L21" s="35"/>
+      <c r="M21" s="35"/>
+      <c r="N21" s="35"/>
+      <c r="O21" s="35"/>
+      <c r="P21" s="35"/>
+      <c r="Q21" s="35"/>
+      <c r="R21" s="35"/>
+      <c r="S21" s="35"/>
+      <c r="T21" s="35"/>
+      <c r="U21" s="35"/>
+      <c r="V21" s="35"/>
+      <c r="W21" s="35"/>
     </row>
     <row r="22" spans="1:23" ht="21" x14ac:dyDescent="0.4">
       <c r="A22" s="19" t="s">
@@ -2307,23 +2307,23 @@
       <c r="H22" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="I22" s="38" t="s">
+      <c r="I22" s="35" t="s">
         <v>147</v>
       </c>
-      <c r="J22" s="38"/>
-      <c r="K22" s="38"/>
-      <c r="L22" s="38"/>
-      <c r="M22" s="38"/>
-      <c r="N22" s="38"/>
-      <c r="O22" s="38"/>
-      <c r="P22" s="38"/>
-      <c r="Q22" s="38"/>
-      <c r="R22" s="38"/>
-      <c r="S22" s="38"/>
-      <c r="T22" s="38"/>
-      <c r="U22" s="38"/>
-      <c r="V22" s="38"/>
-      <c r="W22" s="38"/>
+      <c r="J22" s="35"/>
+      <c r="K22" s="35"/>
+      <c r="L22" s="35"/>
+      <c r="M22" s="35"/>
+      <c r="N22" s="35"/>
+      <c r="O22" s="35"/>
+      <c r="P22" s="35"/>
+      <c r="Q22" s="35"/>
+      <c r="R22" s="35"/>
+      <c r="S22" s="35"/>
+      <c r="T22" s="35"/>
+      <c r="U22" s="35"/>
+      <c r="V22" s="35"/>
+      <c r="W22" s="35"/>
     </row>
     <row r="23" spans="1:23" ht="21" x14ac:dyDescent="0.4">
       <c r="A23" s="19" t="s">
@@ -2351,23 +2351,23 @@
       <c r="H23" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="I23" s="38" t="s">
+      <c r="I23" s="35" t="s">
         <v>139</v>
       </c>
-      <c r="J23" s="38"/>
-      <c r="K23" s="38"/>
-      <c r="L23" s="38"/>
-      <c r="M23" s="38"/>
-      <c r="N23" s="38"/>
-      <c r="O23" s="38"/>
-      <c r="P23" s="38"/>
-      <c r="Q23" s="38"/>
-      <c r="R23" s="38"/>
-      <c r="S23" s="38"/>
-      <c r="T23" s="38"/>
-      <c r="U23" s="38"/>
-      <c r="V23" s="38"/>
-      <c r="W23" s="38"/>
+      <c r="J23" s="35"/>
+      <c r="K23" s="35"/>
+      <c r="L23" s="35"/>
+      <c r="M23" s="35"/>
+      <c r="N23" s="35"/>
+      <c r="O23" s="35"/>
+      <c r="P23" s="35"/>
+      <c r="Q23" s="35"/>
+      <c r="R23" s="35"/>
+      <c r="S23" s="35"/>
+      <c r="T23" s="35"/>
+      <c r="U23" s="35"/>
+      <c r="V23" s="35"/>
+      <c r="W23" s="35"/>
     </row>
     <row r="24" spans="1:23" ht="21" x14ac:dyDescent="0.4">
       <c r="A24" s="19" t="s">
@@ -2395,23 +2395,23 @@
       <c r="H24" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="I24" s="38" t="s">
+      <c r="I24" s="35" t="s">
         <v>149</v>
       </c>
-      <c r="J24" s="38"/>
-      <c r="K24" s="38"/>
-      <c r="L24" s="38"/>
-      <c r="M24" s="38"/>
-      <c r="N24" s="38"/>
-      <c r="O24" s="38"/>
-      <c r="P24" s="38"/>
-      <c r="Q24" s="38"/>
-      <c r="R24" s="38"/>
-      <c r="S24" s="38"/>
-      <c r="T24" s="38"/>
-      <c r="U24" s="38"/>
-      <c r="V24" s="38"/>
-      <c r="W24" s="38"/>
+      <c r="J24" s="35"/>
+      <c r="K24" s="35"/>
+      <c r="L24" s="35"/>
+      <c r="M24" s="35"/>
+      <c r="N24" s="35"/>
+      <c r="O24" s="35"/>
+      <c r="P24" s="35"/>
+      <c r="Q24" s="35"/>
+      <c r="R24" s="35"/>
+      <c r="S24" s="35"/>
+      <c r="T24" s="35"/>
+      <c r="U24" s="35"/>
+      <c r="V24" s="35"/>
+      <c r="W24" s="35"/>
     </row>
     <row r="25" spans="1:23" ht="21" x14ac:dyDescent="0.4">
       <c r="A25" s="19" t="s">
@@ -2439,23 +2439,23 @@
       <c r="H25" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="I25" s="38" t="s">
+      <c r="I25" s="35" t="s">
         <v>151</v>
       </c>
-      <c r="J25" s="38"/>
-      <c r="K25" s="38"/>
-      <c r="L25" s="38"/>
-      <c r="M25" s="38"/>
-      <c r="N25" s="38"/>
-      <c r="O25" s="38"/>
-      <c r="P25" s="38"/>
-      <c r="Q25" s="38"/>
-      <c r="R25" s="38"/>
-      <c r="S25" s="38"/>
-      <c r="T25" s="38"/>
-      <c r="U25" s="38"/>
-      <c r="V25" s="38"/>
-      <c r="W25" s="38"/>
+      <c r="J25" s="35"/>
+      <c r="K25" s="35"/>
+      <c r="L25" s="35"/>
+      <c r="M25" s="35"/>
+      <c r="N25" s="35"/>
+      <c r="O25" s="35"/>
+      <c r="P25" s="35"/>
+      <c r="Q25" s="35"/>
+      <c r="R25" s="35"/>
+      <c r="S25" s="35"/>
+      <c r="T25" s="35"/>
+      <c r="U25" s="35"/>
+      <c r="V25" s="35"/>
+      <c r="W25" s="35"/>
     </row>
     <row r="26" spans="1:23" ht="21" x14ac:dyDescent="0.4">
       <c r="A26" s="19" t="s">
@@ -2483,23 +2483,23 @@
       <c r="H26" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="I26" s="44" t="s">
+      <c r="I26" s="34" t="s">
         <v>178</v>
       </c>
-      <c r="J26" s="44"/>
-      <c r="K26" s="44"/>
-      <c r="L26" s="44"/>
-      <c r="M26" s="44"/>
-      <c r="N26" s="44"/>
-      <c r="O26" s="44"/>
-      <c r="P26" s="44"/>
-      <c r="Q26" s="44"/>
-      <c r="R26" s="44"/>
-      <c r="S26" s="44"/>
-      <c r="T26" s="44"/>
-      <c r="U26" s="44"/>
-      <c r="V26" s="44"/>
-      <c r="W26" s="44"/>
+      <c r="J26" s="34"/>
+      <c r="K26" s="34"/>
+      <c r="L26" s="34"/>
+      <c r="M26" s="34"/>
+      <c r="N26" s="34"/>
+      <c r="O26" s="34"/>
+      <c r="P26" s="34"/>
+      <c r="Q26" s="34"/>
+      <c r="R26" s="34"/>
+      <c r="S26" s="34"/>
+      <c r="T26" s="34"/>
+      <c r="U26" s="34"/>
+      <c r="V26" s="34"/>
+      <c r="W26" s="34"/>
     </row>
     <row r="27" spans="1:23" ht="21" x14ac:dyDescent="0.4">
       <c r="A27" s="19" t="s">
@@ -2527,23 +2527,23 @@
       <c r="H27" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="I27" s="44" t="s">
+      <c r="I27" s="34" t="s">
         <v>180</v>
       </c>
-      <c r="J27" s="44"/>
-      <c r="K27" s="44"/>
-      <c r="L27" s="44"/>
-      <c r="M27" s="44"/>
-      <c r="N27" s="44"/>
-      <c r="O27" s="44"/>
-      <c r="P27" s="44"/>
-      <c r="Q27" s="44"/>
-      <c r="R27" s="44"/>
-      <c r="S27" s="44"/>
-      <c r="T27" s="44"/>
-      <c r="U27" s="44"/>
-      <c r="V27" s="44"/>
-      <c r="W27" s="44"/>
+      <c r="J27" s="34"/>
+      <c r="K27" s="34"/>
+      <c r="L27" s="34"/>
+      <c r="M27" s="34"/>
+      <c r="N27" s="34"/>
+      <c r="O27" s="34"/>
+      <c r="P27" s="34"/>
+      <c r="Q27" s="34"/>
+      <c r="R27" s="34"/>
+      <c r="S27" s="34"/>
+      <c r="T27" s="34"/>
+      <c r="U27" s="34"/>
+      <c r="V27" s="34"/>
+      <c r="W27" s="34"/>
     </row>
     <row r="28" spans="1:23" ht="21" x14ac:dyDescent="0.4">
       <c r="A28" s="19" t="s">
@@ -2571,23 +2571,23 @@
       <c r="H28" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="I28" s="38" t="s">
+      <c r="I28" s="35" t="s">
         <v>153</v>
       </c>
-      <c r="J28" s="38"/>
-      <c r="K28" s="38"/>
-      <c r="L28" s="38"/>
-      <c r="M28" s="38"/>
-      <c r="N28" s="38"/>
-      <c r="O28" s="38"/>
-      <c r="P28" s="38"/>
-      <c r="Q28" s="38"/>
-      <c r="R28" s="38"/>
-      <c r="S28" s="38"/>
-      <c r="T28" s="38"/>
-      <c r="U28" s="38"/>
-      <c r="V28" s="38"/>
-      <c r="W28" s="38"/>
+      <c r="J28" s="35"/>
+      <c r="K28" s="35"/>
+      <c r="L28" s="35"/>
+      <c r="M28" s="35"/>
+      <c r="N28" s="35"/>
+      <c r="O28" s="35"/>
+      <c r="P28" s="35"/>
+      <c r="Q28" s="35"/>
+      <c r="R28" s="35"/>
+      <c r="S28" s="35"/>
+      <c r="T28" s="35"/>
+      <c r="U28" s="35"/>
+      <c r="V28" s="35"/>
+      <c r="W28" s="35"/>
     </row>
     <row r="29" spans="1:23" ht="21" x14ac:dyDescent="0.4">
       <c r="A29" s="19" t="s">
@@ -2615,23 +2615,23 @@
       <c r="H29" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="I29" s="44" t="s">
+      <c r="I29" s="34" t="s">
         <v>182</v>
       </c>
-      <c r="J29" s="44"/>
-      <c r="K29" s="44"/>
-      <c r="L29" s="44"/>
-      <c r="M29" s="44"/>
-      <c r="N29" s="44"/>
-      <c r="O29" s="44"/>
-      <c r="P29" s="44"/>
-      <c r="Q29" s="44"/>
-      <c r="R29" s="44"/>
-      <c r="S29" s="44"/>
-      <c r="T29" s="44"/>
-      <c r="U29" s="44"/>
-      <c r="V29" s="44"/>
-      <c r="W29" s="44"/>
+      <c r="J29" s="34"/>
+      <c r="K29" s="34"/>
+      <c r="L29" s="34"/>
+      <c r="M29" s="34"/>
+      <c r="N29" s="34"/>
+      <c r="O29" s="34"/>
+      <c r="P29" s="34"/>
+      <c r="Q29" s="34"/>
+      <c r="R29" s="34"/>
+      <c r="S29" s="34"/>
+      <c r="T29" s="34"/>
+      <c r="U29" s="34"/>
+      <c r="V29" s="34"/>
+      <c r="W29" s="34"/>
     </row>
     <row r="30" spans="1:23" ht="21" x14ac:dyDescent="0.4">
       <c r="A30" s="19" t="s">
@@ -2659,23 +2659,23 @@
       <c r="H30" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="I30" s="38" t="s">
+      <c r="I30" s="35" t="s">
         <v>155</v>
       </c>
-      <c r="J30" s="38"/>
-      <c r="K30" s="38"/>
-      <c r="L30" s="38"/>
-      <c r="M30" s="38"/>
-      <c r="N30" s="38"/>
-      <c r="O30" s="38"/>
-      <c r="P30" s="38"/>
-      <c r="Q30" s="38"/>
-      <c r="R30" s="38"/>
-      <c r="S30" s="38"/>
-      <c r="T30" s="38"/>
-      <c r="U30" s="38"/>
-      <c r="V30" s="38"/>
-      <c r="W30" s="38"/>
+      <c r="J30" s="35"/>
+      <c r="K30" s="35"/>
+      <c r="L30" s="35"/>
+      <c r="M30" s="35"/>
+      <c r="N30" s="35"/>
+      <c r="O30" s="35"/>
+      <c r="P30" s="35"/>
+      <c r="Q30" s="35"/>
+      <c r="R30" s="35"/>
+      <c r="S30" s="35"/>
+      <c r="T30" s="35"/>
+      <c r="U30" s="35"/>
+      <c r="V30" s="35"/>
+      <c r="W30" s="35"/>
     </row>
     <row r="31" spans="1:23" ht="21" x14ac:dyDescent="0.4">
       <c r="A31" s="19" t="s">
@@ -2703,23 +2703,23 @@
       <c r="H31" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="I31" s="38" t="s">
+      <c r="I31" s="35" t="s">
         <v>156</v>
       </c>
-      <c r="J31" s="38"/>
-      <c r="K31" s="38"/>
-      <c r="L31" s="38"/>
-      <c r="M31" s="38"/>
-      <c r="N31" s="38"/>
-      <c r="O31" s="38"/>
-      <c r="P31" s="38"/>
-      <c r="Q31" s="38"/>
-      <c r="R31" s="38"/>
-      <c r="S31" s="38"/>
-      <c r="T31" s="38"/>
-      <c r="U31" s="38"/>
-      <c r="V31" s="38"/>
-      <c r="W31" s="38"/>
+      <c r="J31" s="35"/>
+      <c r="K31" s="35"/>
+      <c r="L31" s="35"/>
+      <c r="M31" s="35"/>
+      <c r="N31" s="35"/>
+      <c r="O31" s="35"/>
+      <c r="P31" s="35"/>
+      <c r="Q31" s="35"/>
+      <c r="R31" s="35"/>
+      <c r="S31" s="35"/>
+      <c r="T31" s="35"/>
+      <c r="U31" s="35"/>
+      <c r="V31" s="35"/>
+      <c r="W31" s="35"/>
     </row>
     <row r="32" spans="1:23" ht="21" x14ac:dyDescent="0.4">
       <c r="A32" s="21" t="s">
@@ -2747,23 +2747,23 @@
       <c r="H32" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="I32" s="42" t="s">
+      <c r="I32" s="39" t="s">
         <v>111</v>
       </c>
-      <c r="J32" s="43"/>
-      <c r="K32" s="43"/>
-      <c r="L32" s="43"/>
-      <c r="M32" s="43"/>
-      <c r="N32" s="43"/>
-      <c r="O32" s="43"/>
-      <c r="P32" s="43"/>
-      <c r="Q32" s="43"/>
-      <c r="R32" s="43"/>
-      <c r="S32" s="43"/>
-      <c r="T32" s="43"/>
-      <c r="U32" s="43"/>
-      <c r="V32" s="43"/>
-      <c r="W32" s="43"/>
+      <c r="J32" s="40"/>
+      <c r="K32" s="40"/>
+      <c r="L32" s="40"/>
+      <c r="M32" s="40"/>
+      <c r="N32" s="40"/>
+      <c r="O32" s="40"/>
+      <c r="P32" s="40"/>
+      <c r="Q32" s="40"/>
+      <c r="R32" s="40"/>
+      <c r="S32" s="40"/>
+      <c r="T32" s="40"/>
+      <c r="U32" s="40"/>
+      <c r="V32" s="40"/>
+      <c r="W32" s="40"/>
     </row>
     <row r="33" spans="1:23" ht="21" x14ac:dyDescent="0.4">
       <c r="A33" s="19" t="s">
@@ -2790,23 +2790,23 @@
       <c r="H33" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="I33" s="38" t="s">
+      <c r="I33" s="35" t="s">
         <v>158</v>
       </c>
-      <c r="J33" s="38"/>
-      <c r="K33" s="38"/>
-      <c r="L33" s="38"/>
-      <c r="M33" s="38"/>
-      <c r="N33" s="38"/>
-      <c r="O33" s="38"/>
-      <c r="P33" s="38"/>
-      <c r="Q33" s="38"/>
-      <c r="R33" s="38"/>
-      <c r="S33" s="38"/>
-      <c r="T33" s="38"/>
-      <c r="U33" s="38"/>
-      <c r="V33" s="38"/>
-      <c r="W33" s="38"/>
+      <c r="J33" s="35"/>
+      <c r="K33" s="35"/>
+      <c r="L33" s="35"/>
+      <c r="M33" s="35"/>
+      <c r="N33" s="35"/>
+      <c r="O33" s="35"/>
+      <c r="P33" s="35"/>
+      <c r="Q33" s="35"/>
+      <c r="R33" s="35"/>
+      <c r="S33" s="35"/>
+      <c r="T33" s="35"/>
+      <c r="U33" s="35"/>
+      <c r="V33" s="35"/>
+      <c r="W33" s="35"/>
     </row>
     <row r="34" spans="1:23" ht="21" x14ac:dyDescent="0.4">
       <c r="A34" s="21" t="s">
@@ -2834,23 +2834,23 @@
       <c r="H34" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="I34" s="35" t="s">
+      <c r="I34" s="41" t="s">
         <v>111</v>
       </c>
-      <c r="J34" s="35"/>
-      <c r="K34" s="35"/>
-      <c r="L34" s="35"/>
-      <c r="M34" s="35"/>
-      <c r="N34" s="35"/>
-      <c r="O34" s="35"/>
-      <c r="P34" s="35"/>
-      <c r="Q34" s="35"/>
-      <c r="R34" s="35"/>
-      <c r="S34" s="35"/>
-      <c r="T34" s="35"/>
-      <c r="U34" s="35"/>
-      <c r="V34" s="35"/>
-      <c r="W34" s="35"/>
+      <c r="J34" s="41"/>
+      <c r="K34" s="41"/>
+      <c r="L34" s="41"/>
+      <c r="M34" s="41"/>
+      <c r="N34" s="41"/>
+      <c r="O34" s="41"/>
+      <c r="P34" s="41"/>
+      <c r="Q34" s="41"/>
+      <c r="R34" s="41"/>
+      <c r="S34" s="41"/>
+      <c r="T34" s="41"/>
+      <c r="U34" s="41"/>
+      <c r="V34" s="41"/>
+      <c r="W34" s="41"/>
     </row>
     <row r="35" spans="1:23" ht="21" x14ac:dyDescent="0.4">
       <c r="A35" s="19" t="s">
@@ -2878,23 +2878,23 @@
       <c r="H35" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="I35" s="38" t="s">
+      <c r="I35" s="35" t="s">
         <v>161</v>
       </c>
-      <c r="J35" s="38"/>
-      <c r="K35" s="38"/>
-      <c r="L35" s="38"/>
-      <c r="M35" s="38"/>
-      <c r="N35" s="38"/>
-      <c r="O35" s="38"/>
-      <c r="P35" s="38"/>
-      <c r="Q35" s="38"/>
-      <c r="R35" s="38"/>
-      <c r="S35" s="38"/>
-      <c r="T35" s="38"/>
-      <c r="U35" s="38"/>
-      <c r="V35" s="38"/>
-      <c r="W35" s="38"/>
+      <c r="J35" s="35"/>
+      <c r="K35" s="35"/>
+      <c r="L35" s="35"/>
+      <c r="M35" s="35"/>
+      <c r="N35" s="35"/>
+      <c r="O35" s="35"/>
+      <c r="P35" s="35"/>
+      <c r="Q35" s="35"/>
+      <c r="R35" s="35"/>
+      <c r="S35" s="35"/>
+      <c r="T35" s="35"/>
+      <c r="U35" s="35"/>
+      <c r="V35" s="35"/>
+      <c r="W35" s="35"/>
     </row>
     <row r="36" spans="1:23" ht="21" x14ac:dyDescent="0.4">
       <c r="A36" s="21" t="s">
@@ -2922,23 +2922,23 @@
       <c r="H36" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="I36" s="35" t="s">
+      <c r="I36" s="41" t="s">
         <v>111</v>
       </c>
-      <c r="J36" s="35"/>
-      <c r="K36" s="35"/>
-      <c r="L36" s="35"/>
-      <c r="M36" s="35"/>
-      <c r="N36" s="35"/>
-      <c r="O36" s="35"/>
-      <c r="P36" s="35"/>
-      <c r="Q36" s="35"/>
-      <c r="R36" s="35"/>
-      <c r="S36" s="35"/>
-      <c r="T36" s="35"/>
-      <c r="U36" s="35"/>
-      <c r="V36" s="35"/>
-      <c r="W36" s="35"/>
+      <c r="J36" s="41"/>
+      <c r="K36" s="41"/>
+      <c r="L36" s="41"/>
+      <c r="M36" s="41"/>
+      <c r="N36" s="41"/>
+      <c r="O36" s="41"/>
+      <c r="P36" s="41"/>
+      <c r="Q36" s="41"/>
+      <c r="R36" s="41"/>
+      <c r="S36" s="41"/>
+      <c r="T36" s="41"/>
+      <c r="U36" s="41"/>
+      <c r="V36" s="41"/>
+      <c r="W36" s="41"/>
     </row>
     <row r="37" spans="1:23" ht="21" x14ac:dyDescent="0.4">
       <c r="A37" s="19" t="s">
@@ -2966,23 +2966,23 @@
       <c r="H37" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="I37" s="38" t="s">
+      <c r="I37" s="35" t="s">
         <v>163</v>
       </c>
-      <c r="J37" s="38"/>
-      <c r="K37" s="38"/>
-      <c r="L37" s="38"/>
-      <c r="M37" s="38"/>
-      <c r="N37" s="38"/>
-      <c r="O37" s="38"/>
-      <c r="P37" s="38"/>
-      <c r="Q37" s="38"/>
-      <c r="R37" s="38"/>
-      <c r="S37" s="38"/>
-      <c r="T37" s="38"/>
-      <c r="U37" s="38"/>
-      <c r="V37" s="38"/>
-      <c r="W37" s="38"/>
+      <c r="J37" s="35"/>
+      <c r="K37" s="35"/>
+      <c r="L37" s="35"/>
+      <c r="M37" s="35"/>
+      <c r="N37" s="35"/>
+      <c r="O37" s="35"/>
+      <c r="P37" s="35"/>
+      <c r="Q37" s="35"/>
+      <c r="R37" s="35"/>
+      <c r="S37" s="35"/>
+      <c r="T37" s="35"/>
+      <c r="U37" s="35"/>
+      <c r="V37" s="35"/>
+      <c r="W37" s="35"/>
     </row>
     <row r="38" spans="1:23" ht="21" x14ac:dyDescent="0.4">
       <c r="A38" s="21" t="s">
@@ -3010,23 +3010,23 @@
       <c r="H38" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="I38" s="35" t="s">
+      <c r="I38" s="41" t="s">
         <v>111</v>
       </c>
-      <c r="J38" s="35"/>
-      <c r="K38" s="35"/>
-      <c r="L38" s="35"/>
-      <c r="M38" s="35"/>
-      <c r="N38" s="35"/>
-      <c r="O38" s="35"/>
-      <c r="P38" s="35"/>
-      <c r="Q38" s="35"/>
-      <c r="R38" s="35"/>
-      <c r="S38" s="35"/>
-      <c r="T38" s="35"/>
-      <c r="U38" s="35"/>
-      <c r="V38" s="35"/>
-      <c r="W38" s="35"/>
+      <c r="J38" s="41"/>
+      <c r="K38" s="41"/>
+      <c r="L38" s="41"/>
+      <c r="M38" s="41"/>
+      <c r="N38" s="41"/>
+      <c r="O38" s="41"/>
+      <c r="P38" s="41"/>
+      <c r="Q38" s="41"/>
+      <c r="R38" s="41"/>
+      <c r="S38" s="41"/>
+      <c r="T38" s="41"/>
+      <c r="U38" s="41"/>
+      <c r="V38" s="41"/>
+      <c r="W38" s="41"/>
     </row>
     <row r="39" spans="1:23" ht="21" x14ac:dyDescent="0.4">
       <c r="A39" s="21" t="s">
@@ -3054,23 +3054,23 @@
       <c r="H39" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="I39" s="35" t="s">
+      <c r="I39" s="41" t="s">
         <v>111</v>
       </c>
-      <c r="J39" s="35"/>
-      <c r="K39" s="35"/>
-      <c r="L39" s="35"/>
-      <c r="M39" s="35"/>
-      <c r="N39" s="35"/>
-      <c r="O39" s="35"/>
-      <c r="P39" s="35"/>
-      <c r="Q39" s="35"/>
-      <c r="R39" s="35"/>
-      <c r="S39" s="35"/>
-      <c r="T39" s="35"/>
-      <c r="U39" s="35"/>
-      <c r="V39" s="35"/>
-      <c r="W39" s="35"/>
+      <c r="J39" s="41"/>
+      <c r="K39" s="41"/>
+      <c r="L39" s="41"/>
+      <c r="M39" s="41"/>
+      <c r="N39" s="41"/>
+      <c r="O39" s="41"/>
+      <c r="P39" s="41"/>
+      <c r="Q39" s="41"/>
+      <c r="R39" s="41"/>
+      <c r="S39" s="41"/>
+      <c r="T39" s="41"/>
+      <c r="U39" s="41"/>
+      <c r="V39" s="41"/>
+      <c r="W39" s="41"/>
     </row>
     <row r="40" spans="1:23" ht="21" x14ac:dyDescent="0.4">
       <c r="A40" s="19" t="s">
@@ -3098,23 +3098,23 @@
       <c r="H40" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="I40" s="38" t="s">
+      <c r="I40" s="35" t="s">
         <v>165</v>
       </c>
-      <c r="J40" s="38"/>
-      <c r="K40" s="38"/>
-      <c r="L40" s="38"/>
-      <c r="M40" s="38"/>
-      <c r="N40" s="38"/>
-      <c r="O40" s="38"/>
-      <c r="P40" s="38"/>
-      <c r="Q40" s="38"/>
-      <c r="R40" s="38"/>
-      <c r="S40" s="38"/>
-      <c r="T40" s="38"/>
-      <c r="U40" s="38"/>
-      <c r="V40" s="38"/>
-      <c r="W40" s="38"/>
+      <c r="J40" s="35"/>
+      <c r="K40" s="35"/>
+      <c r="L40" s="35"/>
+      <c r="M40" s="35"/>
+      <c r="N40" s="35"/>
+      <c r="O40" s="35"/>
+      <c r="P40" s="35"/>
+      <c r="Q40" s="35"/>
+      <c r="R40" s="35"/>
+      <c r="S40" s="35"/>
+      <c r="T40" s="35"/>
+      <c r="U40" s="35"/>
+      <c r="V40" s="35"/>
+      <c r="W40" s="35"/>
     </row>
     <row r="41" spans="1:23" ht="21" x14ac:dyDescent="0.4">
       <c r="A41" s="20" t="s">
@@ -3142,23 +3142,23 @@
       <c r="H41" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="I41" s="36" t="s">
+      <c r="I41" s="45" t="s">
         <v>194</v>
       </c>
-      <c r="J41" s="37"/>
-      <c r="K41" s="37"/>
-      <c r="L41" s="37"/>
-      <c r="M41" s="37"/>
-      <c r="N41" s="37"/>
-      <c r="O41" s="37"/>
-      <c r="P41" s="37"/>
-      <c r="Q41" s="37"/>
-      <c r="R41" s="37"/>
-      <c r="S41" s="37"/>
-      <c r="T41" s="37"/>
-      <c r="U41" s="37"/>
-      <c r="V41" s="37"/>
-      <c r="W41" s="37"/>
+      <c r="J41" s="46"/>
+      <c r="K41" s="46"/>
+      <c r="L41" s="46"/>
+      <c r="M41" s="46"/>
+      <c r="N41" s="46"/>
+      <c r="O41" s="46"/>
+      <c r="P41" s="46"/>
+      <c r="Q41" s="46"/>
+      <c r="R41" s="46"/>
+      <c r="S41" s="46"/>
+      <c r="T41" s="46"/>
+      <c r="U41" s="46"/>
+      <c r="V41" s="46"/>
+      <c r="W41" s="46"/>
     </row>
     <row r="42" spans="1:23" ht="21" x14ac:dyDescent="0.4">
       <c r="A42" s="20" t="s">
@@ -3186,23 +3186,23 @@
       <c r="H42" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="I42" s="36" t="s">
+      <c r="I42" s="45" t="s">
         <v>189</v>
       </c>
-      <c r="J42" s="37"/>
-      <c r="K42" s="37"/>
-      <c r="L42" s="37"/>
-      <c r="M42" s="37"/>
-      <c r="N42" s="37"/>
-      <c r="O42" s="37"/>
-      <c r="P42" s="37"/>
-      <c r="Q42" s="37"/>
-      <c r="R42" s="37"/>
-      <c r="S42" s="37"/>
-      <c r="T42" s="37"/>
-      <c r="U42" s="37"/>
-      <c r="V42" s="37"/>
-      <c r="W42" s="37"/>
+      <c r="J42" s="46"/>
+      <c r="K42" s="46"/>
+      <c r="L42" s="46"/>
+      <c r="M42" s="46"/>
+      <c r="N42" s="46"/>
+      <c r="O42" s="46"/>
+      <c r="P42" s="46"/>
+      <c r="Q42" s="46"/>
+      <c r="R42" s="46"/>
+      <c r="S42" s="46"/>
+      <c r="T42" s="46"/>
+      <c r="U42" s="46"/>
+      <c r="V42" s="46"/>
+      <c r="W42" s="46"/>
     </row>
     <row r="43" spans="1:23" ht="21" x14ac:dyDescent="0.4">
       <c r="A43" s="20" t="s">
@@ -3230,23 +3230,23 @@
       <c r="H43" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="I43" s="36" t="s">
+      <c r="I43" s="45" t="s">
         <v>185</v>
       </c>
-      <c r="J43" s="37"/>
-      <c r="K43" s="37"/>
-      <c r="L43" s="37"/>
-      <c r="M43" s="37"/>
-      <c r="N43" s="37"/>
-      <c r="O43" s="37"/>
-      <c r="P43" s="37"/>
-      <c r="Q43" s="37"/>
-      <c r="R43" s="37"/>
-      <c r="S43" s="37"/>
-      <c r="T43" s="37"/>
-      <c r="U43" s="37"/>
-      <c r="V43" s="37"/>
-      <c r="W43" s="37"/>
+      <c r="J43" s="46"/>
+      <c r="K43" s="46"/>
+      <c r="L43" s="46"/>
+      <c r="M43" s="46"/>
+      <c r="N43" s="46"/>
+      <c r="O43" s="46"/>
+      <c r="P43" s="46"/>
+      <c r="Q43" s="46"/>
+      <c r="R43" s="46"/>
+      <c r="S43" s="46"/>
+      <c r="T43" s="46"/>
+      <c r="U43" s="46"/>
+      <c r="V43" s="46"/>
+      <c r="W43" s="46"/>
     </row>
     <row r="44" spans="1:23" ht="21" x14ac:dyDescent="0.4">
       <c r="A44" s="20" t="s">
@@ -3274,23 +3274,23 @@
       <c r="H44" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="I44" s="36" t="s">
+      <c r="I44" s="45" t="s">
         <v>187</v>
       </c>
-      <c r="J44" s="37"/>
-      <c r="K44" s="37"/>
-      <c r="L44" s="37"/>
-      <c r="M44" s="37"/>
-      <c r="N44" s="37"/>
-      <c r="O44" s="37"/>
-      <c r="P44" s="37"/>
-      <c r="Q44" s="37"/>
-      <c r="R44" s="37"/>
-      <c r="S44" s="37"/>
-      <c r="T44" s="37"/>
-      <c r="U44" s="37"/>
-      <c r="V44" s="37"/>
-      <c r="W44" s="37"/>
+      <c r="J44" s="46"/>
+      <c r="K44" s="46"/>
+      <c r="L44" s="46"/>
+      <c r="M44" s="46"/>
+      <c r="N44" s="46"/>
+      <c r="O44" s="46"/>
+      <c r="P44" s="46"/>
+      <c r="Q44" s="46"/>
+      <c r="R44" s="46"/>
+      <c r="S44" s="46"/>
+      <c r="T44" s="46"/>
+      <c r="U44" s="46"/>
+      <c r="V44" s="46"/>
+      <c r="W44" s="46"/>
     </row>
     <row r="45" spans="1:23" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A45" s="26" t="s">
@@ -3315,51 +3315,37 @@
       <c r="G45" s="15">
         <v>2684410000</v>
       </c>
-      <c r="H45" s="46" t="s">
+      <c r="H45" s="32" t="s">
         <v>117</v>
       </c>
-      <c r="I45" s="32" t="s">
+      <c r="I45" s="42" t="s">
         <v>192</v>
       </c>
-      <c r="J45" s="33"/>
-      <c r="K45" s="33"/>
-      <c r="L45" s="33"/>
-      <c r="M45" s="33"/>
-      <c r="N45" s="33"/>
-      <c r="O45" s="33"/>
-      <c r="P45" s="33"/>
-      <c r="Q45" s="33"/>
-      <c r="R45" s="33"/>
-      <c r="S45" s="33"/>
-      <c r="T45" s="33"/>
-      <c r="U45" s="33"/>
-      <c r="V45" s="33"/>
-      <c r="W45" s="34"/>
+      <c r="J45" s="43"/>
+      <c r="K45" s="43"/>
+      <c r="L45" s="43"/>
+      <c r="M45" s="43"/>
+      <c r="N45" s="43"/>
+      <c r="O45" s="43"/>
+      <c r="P45" s="43"/>
+      <c r="Q45" s="43"/>
+      <c r="R45" s="43"/>
+      <c r="S45" s="43"/>
+      <c r="T45" s="43"/>
+      <c r="U45" s="43"/>
+      <c r="V45" s="43"/>
+      <c r="W45" s="44"/>
     </row>
     <row r="46" spans="1:23" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="I4:W4"/>
-    <mergeCell ref="I8:W8"/>
-    <mergeCell ref="I5:W5"/>
-    <mergeCell ref="I6:W6"/>
-    <mergeCell ref="I7:W7"/>
-    <mergeCell ref="I9:W9"/>
-    <mergeCell ref="I10:W10"/>
-    <mergeCell ref="I11:W11"/>
-    <mergeCell ref="I12:W12"/>
-    <mergeCell ref="I13:W13"/>
-    <mergeCell ref="I14:W14"/>
-    <mergeCell ref="I15:W15"/>
-    <mergeCell ref="I16:W16"/>
-    <mergeCell ref="I17:W17"/>
-    <mergeCell ref="I18:W18"/>
-    <mergeCell ref="I28:W28"/>
-    <mergeCell ref="I19:W19"/>
-    <mergeCell ref="I20:W20"/>
-    <mergeCell ref="I21:W21"/>
-    <mergeCell ref="I22:W22"/>
-    <mergeCell ref="I23:W23"/>
+    <mergeCell ref="I45:W45"/>
+    <mergeCell ref="I38:W38"/>
+    <mergeCell ref="I39:W39"/>
+    <mergeCell ref="I41:W41"/>
+    <mergeCell ref="I42:W42"/>
+    <mergeCell ref="I44:W44"/>
+    <mergeCell ref="I43:W43"/>
     <mergeCell ref="I37:W37"/>
     <mergeCell ref="I40:W40"/>
     <mergeCell ref="A1:W2"/>
@@ -3376,13 +3362,27 @@
     <mergeCell ref="I25:W25"/>
     <mergeCell ref="I26:W26"/>
     <mergeCell ref="I27:W27"/>
-    <mergeCell ref="I45:W45"/>
-    <mergeCell ref="I38:W38"/>
-    <mergeCell ref="I39:W39"/>
-    <mergeCell ref="I41:W41"/>
-    <mergeCell ref="I42:W42"/>
-    <mergeCell ref="I44:W44"/>
-    <mergeCell ref="I43:W43"/>
+    <mergeCell ref="I28:W28"/>
+    <mergeCell ref="I19:W19"/>
+    <mergeCell ref="I20:W20"/>
+    <mergeCell ref="I21:W21"/>
+    <mergeCell ref="I22:W22"/>
+    <mergeCell ref="I23:W23"/>
+    <mergeCell ref="I14:W14"/>
+    <mergeCell ref="I15:W15"/>
+    <mergeCell ref="I16:W16"/>
+    <mergeCell ref="I17:W17"/>
+    <mergeCell ref="I18:W18"/>
+    <mergeCell ref="I9:W9"/>
+    <mergeCell ref="I10:W10"/>
+    <mergeCell ref="I11:W11"/>
+    <mergeCell ref="I12:W12"/>
+    <mergeCell ref="I13:W13"/>
+    <mergeCell ref="I4:W4"/>
+    <mergeCell ref="I8:W8"/>
+    <mergeCell ref="I5:W5"/>
+    <mergeCell ref="I6:W6"/>
+    <mergeCell ref="I7:W7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="I6" r:id="rId1" xr:uid="{6D2F8233-BCF0-4700-BC9D-74AD8B3FB611}"/>
@@ -3419,6 +3419,7 @@
     <hyperlink ref="I45" r:id="rId32" xr:uid="{C59E3553-42B0-4FAE-8AA5-E41A5F168A97}"/>
     <hyperlink ref="I42" r:id="rId33" xr:uid="{35BDF215-E757-48B6-8602-B3A87E65A509}"/>
     <hyperlink ref="I41" r:id="rId34" xr:uid="{2C11E966-9BB8-4365-8D1F-3C273F5636D8}"/>
+    <hyperlink ref="I16" r:id="rId35" xr:uid="{90F83A89-A36E-4F76-9AC9-AFEEBDCD725E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>